<commit_message>
- Moved toUnixTimestamp static function to XLSReader - Updated sample.php to show usage of toUnixTimestamp and to improve readability
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="123820"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19140" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380"/>
   </bookViews>
   <sheets>
     <sheet name="Source Data" sheetId="1" r:id="rId1"/>
     <sheet name="By Product" sheetId="6" r:id="rId2"/>
     <sheet name="By Product-Customer" sheetId="7" r:id="rId3"/>
     <sheet name="By Product-Customer Filtered" sheetId="8" r:id="rId4"/>
+    <sheet name="Dates" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <webPublishing codePage="1252"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -380,7 +386,7 @@
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,6 +398,22 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -427,10 +449,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -450,23 +476,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -477,7 +496,7 @@
       <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2974,13 +2993,13 @@
     <i>
       <x/>
     </i>
-    <i>
+    <i i="1">
       <x v="1"/>
     </i>
-    <i>
+    <i i="2">
       <x v="2"/>
     </i>
-    <i>
+    <i i="3">
       <x v="3"/>
     </i>
   </colItems>
@@ -2991,7 +3010,7 @@
     <dataField name="Sum of Qtr 4" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="6">
+    <format dxfId="2">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4">
@@ -3258,13 +3277,13 @@
     <i>
       <x/>
     </i>
-    <i>
+    <i i="1">
       <x v="1"/>
     </i>
-    <i>
+    <i i="2">
       <x v="2"/>
     </i>
-    <i>
+    <i i="3">
       <x v="3"/>
     </i>
   </colItems>
@@ -3275,7 +3294,7 @@
     <dataField name="Sum of Qtr 4" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="5">
+    <format dxfId="1">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4">
@@ -3475,7 +3494,7 @@
     <dataField name="Sum of Qtr 4" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="4">
+    <format dxfId="0">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4">
@@ -3794,14 +3813,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="6" customWidth="1"/>
-    <col min="2" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.6640625" style="6" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3821,7 +3840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -3841,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -3861,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -3881,7 +3900,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -3901,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -3921,7 +3940,7 @@
         <v>2607.15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -3941,7 +3960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -3961,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -3981,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
@@ -4001,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -4021,7 +4040,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
@@ -4041,7 +4060,7 @@
         <v>789.75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
@@ -4061,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
@@ -4081,7 +4100,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
@@ -4101,7 +4120,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
@@ -4121,7 +4140,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
@@ -4141,7 +4160,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
@@ -4161,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
@@ -4181,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -4201,7 +4220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
@@ -4221,7 +4240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
@@ -4241,7 +4260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
@@ -4261,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="6" t="s">
         <v>25</v>
       </c>
@@ -4281,7 +4300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -4301,7 +4320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="6" t="s">
         <v>25</v>
       </c>
@@ -4321,7 +4340,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
@@ -4341,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="6" t="s">
         <v>25</v>
       </c>
@@ -4361,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="6" t="s">
         <v>25</v>
       </c>
@@ -4381,7 +4400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="6" t="s">
         <v>25</v>
       </c>
@@ -4401,7 +4420,7 @@
         <v>55.2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -4421,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="6" t="s">
         <v>25</v>
       </c>
@@ -4441,7 +4460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="6" t="s">
         <v>25</v>
       </c>
@@ -4461,7 +4480,7 @@
         <v>110.4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="6" t="s">
         <v>25</v>
       </c>
@@ -4481,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="6" t="s">
         <v>25</v>
       </c>
@@ -4501,7 +4520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="6" t="s">
         <v>25</v>
       </c>
@@ -4521,7 +4540,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="6" t="s">
         <v>25</v>
       </c>
@@ -4541,7 +4560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="6" t="s">
         <v>25</v>
       </c>
@@ -4561,7 +4580,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="6" t="s">
         <v>38</v>
       </c>
@@ -4581,7 +4600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="6" t="s">
         <v>38</v>
       </c>
@@ -4601,7 +4620,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="6" t="s">
         <v>38</v>
       </c>
@@ -4621,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="6" t="s">
         <v>38</v>
       </c>
@@ -4641,7 +4660,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="6" t="s">
         <v>38</v>
       </c>
@@ -4661,7 +4680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="6" t="s">
         <v>38</v>
       </c>
@@ -4681,7 +4700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="6" t="s">
         <v>38</v>
       </c>
@@ -4701,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="6" t="s">
         <v>38</v>
       </c>
@@ -4721,7 +4740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="6" t="s">
         <v>38</v>
       </c>
@@ -4741,7 +4760,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="6" t="s">
         <v>38</v>
       </c>
@@ -4761,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="6" t="s">
         <v>38</v>
       </c>
@@ -4781,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="6" t="s">
         <v>38</v>
       </c>
@@ -4801,7 +4820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="6" t="s">
         <v>38</v>
       </c>
@@ -4821,7 +4840,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="6" t="s">
         <v>38</v>
       </c>
@@ -4841,7 +4860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="6" t="s">
         <v>38</v>
       </c>
@@ -4861,7 +4880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="6" t="s">
         <v>38</v>
       </c>
@@ -4881,7 +4900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="6" t="s">
         <v>38</v>
       </c>
@@ -4901,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="6" t="s">
         <v>38</v>
       </c>
@@ -4921,7 +4940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="6" t="s">
         <v>38</v>
       </c>
@@ -4941,7 +4960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="6" t="s">
         <v>51</v>
       </c>
@@ -4961,7 +4980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="6" t="s">
         <v>51</v>
       </c>
@@ -4981,7 +5000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="6" t="s">
         <v>51</v>
       </c>
@@ -5001,7 +5020,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="6" t="s">
         <v>51</v>
       </c>
@@ -5021,7 +5040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="6" t="s">
         <v>51</v>
       </c>
@@ -5041,7 +5060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="6" t="s">
         <v>51</v>
       </c>
@@ -5061,7 +5080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="6" t="s">
         <v>51</v>
       </c>
@@ -5081,7 +5100,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="6" t="s">
         <v>51</v>
       </c>
@@ -5101,7 +5120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="6" t="s">
         <v>51</v>
       </c>
@@ -5121,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="6" t="s">
         <v>51</v>
       </c>
@@ -5141,7 +5160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="6" t="s">
         <v>55</v>
       </c>
@@ -5161,7 +5180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" s="6" t="s">
         <v>55</v>
       </c>
@@ -5181,7 +5200,7 @@
         <v>85.4</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" s="6" t="s">
         <v>57</v>
       </c>
@@ -5201,7 +5220,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" s="6" t="s">
         <v>57</v>
       </c>
@@ -5221,7 +5240,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" s="6" t="s">
         <v>57</v>
       </c>
@@ -5241,7 +5260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" s="6" t="s">
         <v>57</v>
       </c>
@@ -5261,7 +5280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" s="6" t="s">
         <v>57</v>
       </c>
@@ -5281,7 +5300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" s="6" t="s">
         <v>57</v>
       </c>
@@ -5301,7 +5320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" s="6" t="s">
         <v>57</v>
       </c>
@@ -5321,7 +5340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" s="6" t="s">
         <v>57</v>
       </c>
@@ -5341,7 +5360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" s="6" t="s">
         <v>57</v>
       </c>
@@ -5361,7 +5380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" s="6" t="s">
         <v>57</v>
       </c>
@@ -5381,7 +5400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" s="6" t="s">
         <v>57</v>
       </c>
@@ -5401,7 +5420,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" s="6" t="s">
         <v>57</v>
       </c>
@@ -5421,7 +5440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" s="6" t="s">
         <v>57</v>
       </c>
@@ -5441,7 +5460,7 @@
         <v>99.75</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" s="6" t="s">
         <v>57</v>
       </c>
@@ -5461,7 +5480,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" s="6" t="s">
         <v>65</v>
       </c>
@@ -5481,7 +5500,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" s="6" t="s">
         <v>65</v>
       </c>
@@ -5501,7 +5520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" s="6" t="s">
         <v>65</v>
       </c>
@@ -5521,7 +5540,7 @@
         <v>35.619999999999997</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="6" t="s">
         <v>65</v>
       </c>
@@ -5541,7 +5560,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="6" t="s">
         <v>65</v>
       </c>
@@ -5561,7 +5580,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="6" t="s">
         <v>65</v>
       </c>
@@ -5581,7 +5600,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="6" t="s">
         <v>65</v>
       </c>
@@ -5601,7 +5620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="6" t="s">
         <v>65</v>
       </c>
@@ -5621,7 +5640,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="6" t="s">
         <v>65</v>
       </c>
@@ -5641,7 +5660,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="6" t="s">
         <v>65</v>
       </c>
@@ -5661,7 +5680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="6" t="s">
         <v>65</v>
       </c>
@@ -5681,7 +5700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="6" t="s">
         <v>65</v>
       </c>
@@ -5701,7 +5720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="6" t="s">
         <v>65</v>
       </c>
@@ -5721,7 +5740,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" s="6" t="s">
         <v>65</v>
       </c>
@@ -5741,7 +5760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98" s="6" t="s">
         <v>65</v>
       </c>
@@ -5761,7 +5780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="6" t="s">
         <v>65</v>
       </c>
@@ -5781,7 +5800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="6" t="s">
         <v>65</v>
       </c>
@@ -5801,7 +5820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101" s="6" t="s">
         <v>65</v>
       </c>
@@ -5821,7 +5840,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="A102" s="6" t="s">
         <v>65</v>
       </c>
@@ -5841,7 +5860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="A103" s="6" t="s">
         <v>65</v>
       </c>
@@ -5861,7 +5880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="A104" s="6" t="s">
         <v>65</v>
       </c>
@@ -5881,7 +5900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="A105" s="6" t="s">
         <v>65</v>
       </c>
@@ -5901,7 +5920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6">
       <c r="A106" s="6" t="s">
         <v>65</v>
       </c>
@@ -5921,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6">
       <c r="A107" s="6" t="s">
         <v>65</v>
       </c>
@@ -5941,7 +5960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6">
       <c r="A108" s="6" t="s">
         <v>72</v>
       </c>
@@ -5961,7 +5980,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6">
       <c r="A109" s="6" t="s">
         <v>72</v>
       </c>
@@ -5981,7 +6000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6">
       <c r="A110" s="6" t="s">
         <v>73</v>
       </c>
@@ -6001,7 +6020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6">
       <c r="A111" s="6" t="s">
         <v>73</v>
       </c>
@@ -6021,7 +6040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6">
       <c r="A112" s="6" t="s">
         <v>73</v>
       </c>
@@ -6041,7 +6060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6">
       <c r="A113" s="6" t="s">
         <v>73</v>
       </c>
@@ -6061,7 +6080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6">
       <c r="A114" s="6" t="s">
         <v>73</v>
       </c>
@@ -6081,7 +6100,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6">
       <c r="A115" s="6" t="s">
         <v>73</v>
       </c>
@@ -6101,7 +6120,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6">
       <c r="A116" s="6" t="s">
         <v>73</v>
       </c>
@@ -6121,7 +6140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6">
       <c r="A117" s="6" t="s">
         <v>73</v>
       </c>
@@ -6141,7 +6160,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6">
       <c r="A118" s="6" t="s">
         <v>73</v>
       </c>
@@ -6161,7 +6180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6">
       <c r="A119" s="6" t="s">
         <v>73</v>
       </c>
@@ -6181,7 +6200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6">
       <c r="A120" s="6" t="s">
         <v>73</v>
       </c>
@@ -6201,7 +6220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6">
       <c r="A121" s="6" t="s">
         <v>78</v>
       </c>
@@ -6221,7 +6240,7 @@
         <v>135.1</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6">
       <c r="A122" s="6" t="s">
         <v>78</v>
       </c>
@@ -6241,7 +6260,7 @@
         <v>96.5</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6">
       <c r="A123" s="6" t="s">
         <v>78</v>
       </c>
@@ -6261,7 +6280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6">
       <c r="A124" s="6" t="s">
         <v>78</v>
       </c>
@@ -6281,7 +6300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6">
       <c r="A125" s="6" t="s">
         <v>78</v>
       </c>
@@ -6301,7 +6320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6">
       <c r="A126" s="6" t="s">
         <v>78</v>
       </c>
@@ -6321,7 +6340,7 @@
         <v>115.8</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6">
       <c r="A127" s="6" t="s">
         <v>78</v>
       </c>
@@ -6341,7 +6360,7 @@
         <v>183.35</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6">
       <c r="A128" s="6" t="s">
         <v>78</v>
       </c>
@@ -6361,7 +6380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6">
       <c r="A129" s="6" t="s">
         <v>78</v>
       </c>
@@ -6381,7 +6400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6">
       <c r="A130" s="6" t="s">
         <v>78</v>
       </c>
@@ -6401,7 +6420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6">
       <c r="A131" s="6" t="s">
         <v>78</v>
       </c>
@@ -6421,7 +6440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6">
       <c r="A132" s="6" t="s">
         <v>78</v>
       </c>
@@ -6441,7 +6460,7 @@
         <v>337.75</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6">
       <c r="A133" s="6" t="s">
         <v>78</v>
       </c>
@@ -6461,7 +6480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6">
       <c r="A134" s="6" t="s">
         <v>78</v>
       </c>
@@ -6481,7 +6500,7 @@
         <v>405.3</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6">
       <c r="A135" s="6" t="s">
         <v>78</v>
       </c>
@@ -6501,7 +6520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6">
       <c r="A136" s="6" t="s">
         <v>78</v>
       </c>
@@ -6521,7 +6540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6">
       <c r="A137" s="6" t="s">
         <v>78</v>
       </c>
@@ -6541,7 +6560,7 @@
         <v>275.02</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6">
       <c r="A138" s="6" t="s">
         <v>78</v>
       </c>
@@ -6561,7 +6580,7 @@
         <v>115.8</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6">
       <c r="A139" s="6" t="s">
         <v>79</v>
       </c>
@@ -6581,7 +6600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6">
       <c r="A140" s="6" t="s">
         <v>79</v>
       </c>
@@ -6601,7 +6620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6">
       <c r="A141" s="6" t="s">
         <v>79</v>
       </c>
@@ -6621,7 +6640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6">
       <c r="A142" s="6" t="s">
         <v>79</v>
       </c>
@@ -6641,7 +6660,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6">
       <c r="A143" s="6" t="s">
         <v>82</v>
       </c>
@@ -6661,7 +6680,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6">
       <c r="A144" s="6" t="s">
         <v>82</v>
       </c>
@@ -6681,7 +6700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6">
       <c r="A145" s="6" t="s">
         <v>82</v>
       </c>
@@ -6701,7 +6720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6">
       <c r="A146" s="6" t="s">
         <v>82</v>
       </c>
@@ -6721,7 +6740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6">
       <c r="A147" s="6" t="s">
         <v>82</v>
       </c>
@@ -6741,7 +6760,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6">
       <c r="A148" s="6" t="s">
         <v>82</v>
       </c>
@@ -6761,7 +6780,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6">
       <c r="A149" s="6" t="s">
         <v>84</v>
       </c>
@@ -6781,7 +6800,7 @@
         <v>199.97</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6">
       <c r="A150" s="6" t="s">
         <v>84</v>
       </c>
@@ -6801,7 +6820,7 @@
         <v>1299.8399999999999</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6">
       <c r="A151" s="6" t="s">
         <v>84</v>
       </c>
@@ -6821,7 +6840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6">
       <c r="A152" s="6" t="s">
         <v>84</v>
       </c>
@@ -6841,7 +6860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6">
       <c r="A153" s="6" t="s">
         <v>84</v>
       </c>
@@ -6861,7 +6880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6">
       <c r="A154" s="6" t="s">
         <v>84</v>
       </c>
@@ -6881,7 +6900,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6">
       <c r="A155" s="6" t="s">
         <v>84</v>
       </c>
@@ -6901,7 +6920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6">
       <c r="A156" s="6" t="s">
         <v>84</v>
       </c>
@@ -6921,7 +6940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6">
       <c r="A157" s="6" t="s">
         <v>84</v>
       </c>
@@ -6941,7 +6960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6">
       <c r="A158" s="6" t="s">
         <v>84</v>
       </c>
@@ -6961,7 +6980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6">
       <c r="A159" s="6" t="s">
         <v>84</v>
       </c>
@@ -6981,7 +7000,7 @@
         <v>1515.6</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6">
       <c r="A160" s="6" t="s">
         <v>84</v>
       </c>
@@ -7001,7 +7020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6">
       <c r="A161" s="6" t="s">
         <v>84</v>
       </c>
@@ -7021,7 +7040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6">
       <c r="A162" s="6" t="s">
         <v>84</v>
       </c>
@@ -7041,7 +7060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6">
       <c r="A163" s="6" t="s">
         <v>84</v>
       </c>
@@ -7061,7 +7080,7 @@
         <v>42.1</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6">
       <c r="A164" s="6" t="s">
         <v>87</v>
       </c>
@@ -7081,7 +7100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6">
       <c r="A165" s="6" t="s">
         <v>87</v>
       </c>
@@ -7101,7 +7120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6">
       <c r="A166" s="6" t="s">
         <v>87</v>
       </c>
@@ -7121,7 +7140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6">
       <c r="A167" s="6" t="s">
         <v>87</v>
       </c>
@@ -7141,7 +7160,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6">
       <c r="A168" s="6" t="s">
         <v>87</v>
       </c>
@@ -7161,7 +7180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6">
       <c r="A169" s="6" t="s">
         <v>87</v>
       </c>
@@ -7181,7 +7200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6">
       <c r="A170" s="6" t="s">
         <v>88</v>
       </c>
@@ -7201,7 +7220,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6">
       <c r="A171" s="6" t="s">
         <v>88</v>
       </c>
@@ -7221,7 +7240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6">
       <c r="A172" s="6" t="s">
         <v>88</v>
       </c>
@@ -7241,7 +7260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6">
       <c r="A173" s="6" t="s">
         <v>88</v>
       </c>
@@ -7261,7 +7280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6">
       <c r="A174" s="6" t="s">
         <v>88</v>
       </c>
@@ -7281,7 +7300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6">
       <c r="A175" s="6" t="s">
         <v>88</v>
       </c>
@@ -7301,7 +7320,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6">
       <c r="A176" s="6" t="s">
         <v>88</v>
       </c>
@@ -7321,7 +7340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6">
       <c r="A177" s="6" t="s">
         <v>88</v>
       </c>
@@ -7341,7 +7360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6">
       <c r="A178" s="6" t="s">
         <v>88</v>
       </c>
@@ -7361,7 +7380,7 @@
         <v>887.4</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6">
       <c r="A179" s="6" t="s">
         <v>88</v>
       </c>
@@ -7381,7 +7400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6">
       <c r="A180" s="6" t="s">
         <v>88</v>
       </c>
@@ -7401,7 +7420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6">
       <c r="A181" s="6" t="s">
         <v>88</v>
       </c>
@@ -7421,7 +7440,7 @@
         <v>243.6</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6">
       <c r="A182" s="6" t="s">
         <v>88</v>
       </c>
@@ -7441,7 +7460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6">
       <c r="A183" s="6" t="s">
         <v>88</v>
       </c>
@@ -7461,7 +7480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6">
       <c r="A184" s="6" t="s">
         <v>88</v>
       </c>
@@ -7481,7 +7500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6">
       <c r="A185" s="6" t="s">
         <v>88</v>
       </c>
@@ -7501,7 +7520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6">
       <c r="A186" s="6" t="s">
         <v>94</v>
       </c>
@@ -7521,7 +7540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6">
       <c r="A187" s="6" t="s">
         <v>94</v>
       </c>
@@ -7541,7 +7560,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6">
       <c r="A188" s="6" t="s">
         <v>94</v>
       </c>
@@ -7561,7 +7580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6">
       <c r="A189" s="6" t="s">
         <v>94</v>
       </c>
@@ -7581,7 +7600,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6">
       <c r="A190" s="6" t="s">
         <v>94</v>
       </c>
@@ -7601,7 +7620,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6">
       <c r="A191" s="6" t="s">
         <v>95</v>
       </c>
@@ -7621,7 +7640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6">
       <c r="A192" s="6" t="s">
         <v>95</v>
       </c>
@@ -7641,7 +7660,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6">
       <c r="A193" s="6" t="s">
         <v>95</v>
       </c>
@@ -7661,7 +7680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6">
       <c r="A194" s="6" t="s">
         <v>95</v>
       </c>
@@ -7681,7 +7700,7 @@
         <v>204.75</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6">
       <c r="A195" s="6" t="s">
         <v>95</v>
       </c>
@@ -7701,7 +7720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6">
       <c r="A196" s="6" t="s">
         <v>95</v>
       </c>
@@ -7721,7 +7740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6">
       <c r="A197" s="6" t="s">
         <v>95</v>
       </c>
@@ -7741,7 +7760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6">
       <c r="A198" s="6" t="s">
         <v>95</v>
       </c>
@@ -7761,7 +7780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6">
       <c r="A199" s="6" t="s">
         <v>97</v>
       </c>
@@ -7781,7 +7800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6">
       <c r="A200" s="6" t="s">
         <v>97</v>
       </c>
@@ -7801,7 +7820,7 @@
         <v>554.4</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6">
       <c r="A201" s="6" t="s">
         <v>97</v>
       </c>
@@ -7821,7 +7840,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6">
       <c r="A202" s="6" t="s">
         <v>97</v>
       </c>
@@ -7841,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6">
       <c r="A203" s="6" t="s">
         <v>97</v>
       </c>
@@ -7861,7 +7880,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6">
       <c r="A204" s="6" t="s">
         <v>97</v>
       </c>
@@ -7881,7 +7900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6">
       <c r="A205" s="6" t="s">
         <v>98</v>
       </c>
@@ -7901,7 +7920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6">
       <c r="A206" s="6" t="s">
         <v>98</v>
       </c>
@@ -7921,7 +7940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6">
       <c r="A207" s="6" t="s">
         <v>98</v>
       </c>
@@ -7941,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6">
       <c r="A208" s="6" t="s">
         <v>98</v>
       </c>
@@ -7961,7 +7980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6">
       <c r="A209" s="6" t="s">
         <v>99</v>
       </c>
@@ -7981,7 +8000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6">
       <c r="A210" s="6" t="s">
         <v>99</v>
       </c>
@@ -8001,7 +8020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6">
       <c r="A211" s="6" t="s">
         <v>99</v>
       </c>
@@ -8021,7 +8040,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6">
       <c r="A212" s="6" t="s">
         <v>99</v>
       </c>
@@ -8041,7 +8060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6">
       <c r="A213" s="6" t="s">
         <v>99</v>
       </c>
@@ -8061,7 +8080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6">
       <c r="A214" s="6" t="s">
         <v>99</v>
       </c>
@@ -8081,7 +8100,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6">
       <c r="A215" s="6" t="s">
         <v>99</v>
       </c>
@@ -8101,7 +8120,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6">
       <c r="A216" s="6" t="s">
         <v>99</v>
       </c>
@@ -8121,7 +8140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6">
       <c r="A217" s="6" t="s">
         <v>99</v>
       </c>
@@ -8141,7 +8160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6">
       <c r="A218" s="6" t="s">
         <v>99</v>
       </c>
@@ -8161,7 +8180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6">
       <c r="A219" s="6" t="s">
         <v>99</v>
       </c>
@@ -8181,7 +8200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6">
       <c r="A220" s="6" t="s">
         <v>99</v>
       </c>
@@ -8201,7 +8220,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6">
       <c r="A221" s="6" t="s">
         <v>99</v>
       </c>
@@ -8221,7 +8240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6">
       <c r="A222" s="6" t="s">
         <v>99</v>
       </c>
@@ -8241,7 +8260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6">
       <c r="A223" s="6" t="s">
         <v>99</v>
       </c>
@@ -8261,7 +8280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6">
       <c r="A224" s="6" t="s">
         <v>99</v>
       </c>
@@ -8281,7 +8300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6">
       <c r="A225" s="6" t="s">
         <v>99</v>
       </c>
@@ -8301,7 +8320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6">
       <c r="A226" s="6" t="s">
         <v>99</v>
       </c>
@@ -8321,7 +8340,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6">
       <c r="A227" s="6" t="s">
         <v>99</v>
       </c>
@@ -8341,7 +8360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6">
       <c r="A228" s="6" t="s">
         <v>99</v>
       </c>
@@ -8361,7 +8380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6">
       <c r="A229" s="6" t="s">
         <v>99</v>
       </c>
@@ -8381,7 +8400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6">
       <c r="A230" s="6" t="s">
         <v>104</v>
       </c>
@@ -8401,7 +8420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6">
       <c r="A231" s="6" t="s">
         <v>104</v>
       </c>
@@ -8421,7 +8440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6">
       <c r="A232" s="6" t="s">
         <v>104</v>
       </c>
@@ -8441,7 +8460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6">
       <c r="A233" s="6" t="s">
         <v>104</v>
       </c>
@@ -8461,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6">
       <c r="A234" s="6" t="s">
         <v>104</v>
       </c>
@@ -8481,7 +8500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6">
       <c r="A235" s="6" t="s">
         <v>104</v>
       </c>
@@ -8501,7 +8520,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6">
       <c r="A236" s="6" t="s">
         <v>104</v>
       </c>
@@ -8521,7 +8540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6">
       <c r="A237" s="6" t="s">
         <v>104</v>
       </c>
@@ -8541,7 +8560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6">
       <c r="A238" s="6" t="s">
         <v>104</v>
       </c>
@@ -8561,7 +8580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6">
       <c r="A239" s="6" t="s">
         <v>104</v>
       </c>
@@ -8581,7 +8600,7 @@
         <v>121.5</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6">
       <c r="A240" s="6" t="s">
         <v>104</v>
       </c>
@@ -8601,7 +8620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6">
       <c r="A241" s="6" t="s">
         <v>104</v>
       </c>
@@ -8621,7 +8640,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6">
       <c r="A242" s="6" t="s">
         <v>104</v>
       </c>
@@ -8641,7 +8660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6">
       <c r="A243" s="6" t="s">
         <v>104</v>
       </c>
@@ -8661,7 +8680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6">
       <c r="A244" s="6" t="s">
         <v>104</v>
       </c>
@@ -8681,7 +8700,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6">
       <c r="A245" s="6" t="s">
         <v>106</v>
       </c>
@@ -8701,7 +8720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6">
       <c r="A246" s="6" t="s">
         <v>106</v>
       </c>
@@ -8721,7 +8740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6">
       <c r="A247" s="6" t="s">
         <v>106</v>
       </c>
@@ -8741,7 +8760,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6">
       <c r="A248" s="6" t="s">
         <v>106</v>
       </c>
@@ -8761,7 +8780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6">
       <c r="A249" s="6" t="s">
         <v>106</v>
       </c>
@@ -8781,7 +8800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6">
       <c r="A250" s="6" t="s">
         <v>106</v>
       </c>
@@ -8801,7 +8820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6">
       <c r="A251" s="6" t="s">
         <v>106</v>
       </c>
@@ -8821,7 +8840,7 @@
         <v>48.3</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6">
       <c r="A252" s="6" t="s">
         <v>106</v>
       </c>
@@ -8841,7 +8860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6">
       <c r="A253" s="6" t="s">
         <v>106</v>
       </c>
@@ -8861,7 +8880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6">
       <c r="A254" s="6" t="s">
         <v>106</v>
       </c>
@@ -8881,7 +8900,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6">
       <c r="A255" s="6" t="s">
         <v>106</v>
       </c>
@@ -8901,7 +8920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6">
       <c r="A256" s="6" t="s">
         <v>106</v>
       </c>
@@ -8921,7 +8940,7 @@
         <v>110.4</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6">
       <c r="A257" s="6" t="s">
         <v>106</v>
       </c>
@@ -8941,7 +8960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6">
       <c r="A258" s="6" t="s">
         <v>106</v>
       </c>
@@ -8961,7 +8980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6">
       <c r="A259" s="6" t="s">
         <v>106</v>
       </c>
@@ -8981,7 +9000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6">
       <c r="A260" s="6" t="s">
         <v>106</v>
       </c>
@@ -9001,7 +9020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6">
       <c r="A261" s="6" t="s">
         <v>106</v>
       </c>
@@ -9021,7 +9040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6">
       <c r="A262" s="6" t="s">
         <v>106</v>
       </c>
@@ -9041,7 +9060,7 @@
         <v>209.76</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6">
       <c r="A263" s="6" t="s">
         <v>107</v>
       </c>
@@ -9061,7 +9080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6">
       <c r="A264" s="6" t="s">
         <v>107</v>
       </c>
@@ -9081,7 +9100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6">
       <c r="A265" s="6" t="s">
         <v>107</v>
       </c>
@@ -9101,7 +9120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6">
       <c r="A266" s="6" t="s">
         <v>107</v>
       </c>
@@ -9121,7 +9140,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6">
       <c r="A267" s="6" t="s">
         <v>107</v>
       </c>
@@ -9141,7 +9160,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6">
       <c r="A268" s="6" t="s">
         <v>107</v>
       </c>
@@ -9161,7 +9180,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6">
       <c r="A269" s="6" t="s">
         <v>107</v>
       </c>
@@ -9181,7 +9200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6">
       <c r="A270" s="6" t="s">
         <v>107</v>
       </c>
@@ -9201,7 +9220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6">
       <c r="A271" s="6" t="s">
         <v>107</v>
       </c>
@@ -9221,7 +9240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6">
       <c r="A272" s="6" t="s">
         <v>109</v>
       </c>
@@ -9241,7 +9260,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6">
       <c r="A273" s="6" t="s">
         <v>109</v>
       </c>
@@ -9261,7 +9280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6">
       <c r="A274" s="6" t="s">
         <v>109</v>
       </c>
@@ -9281,7 +9300,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6">
       <c r="A275" s="6" t="s">
         <v>109</v>
       </c>
@@ -9301,7 +9320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6">
       <c r="A276" s="6" t="s">
         <v>109</v>
       </c>
@@ -9321,7 +9340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6">
       <c r="A277" s="6" t="s">
         <v>109</v>
       </c>
@@ -9341,7 +9360,7 @@
         <v>395.1</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6">
       <c r="A278" s="6" t="s">
         <v>109</v>
       </c>
@@ -9367,7 +9386,12 @@
   </sortState>
   <printOptions gridLines="1"/>
   <pageMargins left="0.35" right="0.35" top="0.75" bottom="0.75" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9379,18 +9403,18 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="B6" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -9407,7 +9431,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -9424,7 +9448,7 @@
         <v>6087.9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -9441,7 +9465,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -9458,7 +9482,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -9475,7 +9499,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -9492,7 +9516,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
         <v>55</v>
       </c>
@@ -9509,7 +9533,7 @@
         <v>85.4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
         <v>57</v>
       </c>
@@ -9526,7 +9550,7 @@
         <v>904.75</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
         <v>65</v>
       </c>
@@ -9543,7 +9567,7 @@
         <v>2681.87</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
         <v>72</v>
       </c>
@@ -9560,7 +9584,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
         <v>73</v>
       </c>
@@ -9577,7 +9601,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>78</v>
       </c>
@@ -9594,7 +9618,7 @@
         <v>1664.62</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>79</v>
       </c>
@@ -9611,7 +9635,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
         <v>82</v>
       </c>
@@ -9628,7 +9652,7 @@
         <v>512.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>84</v>
       </c>
@@ -9645,7 +9669,7 @@
         <v>3899.51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
         <v>87</v>
       </c>
@@ -9662,7 +9686,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
         <v>88</v>
       </c>
@@ -9679,7 +9703,7 @@
         <v>2697</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
         <v>94</v>
       </c>
@@ -9696,7 +9720,7 @@
         <v>2960</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
         <v>95</v>
       </c>
@@ -9713,7 +9737,7 @@
         <v>984.75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
         <v>97</v>
       </c>
@@ -9730,7 +9754,7 @@
         <v>890.4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
         <v>98</v>
       </c>
@@ -9747,7 +9771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
         <v>99</v>
       </c>
@@ -9764,7 +9788,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="4" t="s">
         <v>104</v>
       </c>
@@ -9781,7 +9805,7 @@
         <v>1273.5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
         <v>106</v>
       </c>
@@ -9798,7 +9822,7 @@
         <v>851.46</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
         <v>107</v>
       </c>
@@ -9815,7 +9839,7 @@
         <v>3826.5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
         <v>109</v>
       </c>
@@ -9832,7 +9856,7 @@
         <v>2590.1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="4" t="s">
         <v>108</v>
       </c>
@@ -9851,7 +9875,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9863,19 +9892,19 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="26.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="B6" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -9892,7 +9921,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -9901,7 +9930,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -9918,7 +9947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -9935,7 +9964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -9952,7 +9981,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -9969,7 +9998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -9986,7 +10015,7 @@
         <v>2607.15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -10003,7 +10032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -10020,7 +10049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
@@ -10037,7 +10066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -10054,7 +10083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
@@ -10071,7 +10100,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
@@ -10088,7 +10117,7 @@
         <v>789.75</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
@@ -10105,7 +10134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
@@ -10122,7 +10151,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
@@ -10139,7 +10168,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -10156,7 +10185,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
@@ -10173,7 +10202,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
         <v>51</v>
       </c>
@@ -10190,7 +10219,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
         <v>55</v>
       </c>
@@ -10207,7 +10236,7 @@
         <v>85.4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -10224,7 +10253,7 @@
         <v>904.75</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
         <v>65</v>
       </c>
@@ -10241,7 +10270,7 @@
         <v>2681.87</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="4" t="s">
         <v>72</v>
       </c>
@@ -10258,7 +10287,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
         <v>73</v>
       </c>
@@ -10275,7 +10304,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
         <v>78</v>
       </c>
@@ -10292,7 +10321,7 @@
         <v>1664.62</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
         <v>79</v>
       </c>
@@ -10309,7 +10338,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="4" t="s">
         <v>82</v>
       </c>
@@ -10326,7 +10355,7 @@
         <v>512.5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="4" t="s">
         <v>84</v>
       </c>
@@ -10343,7 +10372,7 @@
         <v>3899.51</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="4" t="s">
         <v>87</v>
       </c>
@@ -10360,7 +10389,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="4" t="s">
         <v>88</v>
       </c>
@@ -10377,7 +10406,7 @@
         <v>2697</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="4" t="s">
         <v>94</v>
       </c>
@@ -10394,7 +10423,7 @@
         <v>2960</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="4" t="s">
         <v>95</v>
       </c>
@@ -10411,7 +10440,7 @@
         <v>984.75</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="4" t="s">
         <v>97</v>
       </c>
@@ -10428,7 +10457,7 @@
         <v>890.4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="4" t="s">
         <v>98</v>
       </c>
@@ -10445,7 +10474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="4" t="s">
         <v>99</v>
       </c>
@@ -10462,7 +10491,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="4" t="s">
         <v>104</v>
       </c>
@@ -10479,7 +10508,7 @@
         <v>1273.5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="4" t="s">
         <v>106</v>
       </c>
@@ -10496,7 +10525,7 @@
         <v>851.46</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="4" t="s">
         <v>107</v>
       </c>
@@ -10513,7 +10542,7 @@
         <v>3826.5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="4" t="s">
         <v>109</v>
       </c>
@@ -10530,7 +10559,7 @@
         <v>2590.1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="4" t="s">
         <v>108</v>
       </c>
@@ -10549,7 +10578,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10561,23 +10595,23 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="B6" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -10594,7 +10628,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -10611,7 +10645,7 @@
         <v>6087.9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -10628,7 +10662,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>38</v>
       </c>
@@ -10645,7 +10679,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>73</v>
       </c>
@@ -10662,7 +10696,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>84</v>
       </c>
@@ -10679,7 +10713,7 @@
         <v>3899.5099999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
         <v>87</v>
       </c>
@@ -10696,7 +10730,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
         <v>88</v>
       </c>
@@ -10713,7 +10747,7 @@
         <v>2697</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
         <v>99</v>
       </c>
@@ -10730,7 +10764,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
         <v>104</v>
       </c>
@@ -10747,7 +10781,7 @@
         <v>1273.5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
         <v>109</v>
       </c>
@@ -10764,7 +10798,7 @@
         <v>2590.1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>108</v>
       </c>
@@ -10783,6 +10817,329 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="11">
+        <v>41030</v>
+      </c>
+      <c r="B1">
+        <f ca="1">RANDBETWEEN(0,100)</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="11">
+        <f>A1+1</f>
+        <v>41031</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B30" ca="1" si="0">RANDBETWEEN(0,100)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="11">
+        <f t="shared" ref="A3:A30" si="1">A2+1</f>
+        <v>41032</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="11">
+        <f t="shared" si="1"/>
+        <v>41033</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11">
+        <f t="shared" si="1"/>
+        <v>41034</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="11">
+        <f t="shared" si="1"/>
+        <v>41035</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="11">
+        <f t="shared" si="1"/>
+        <v>41036</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="11">
+        <f t="shared" si="1"/>
+        <v>41037</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="11">
+        <f t="shared" si="1"/>
+        <v>41038</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="11">
+        <f t="shared" si="1"/>
+        <v>41039</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="11">
+        <f t="shared" si="1"/>
+        <v>41040</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="11">
+        <f t="shared" si="1"/>
+        <v>41041</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="11">
+        <f t="shared" si="1"/>
+        <v>41042</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="11">
+        <f t="shared" si="1"/>
+        <v>41043</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="11">
+        <f t="shared" si="1"/>
+        <v>41044</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="0"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="11">
+        <f t="shared" si="1"/>
+        <v>41045</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="11">
+        <f t="shared" si="1"/>
+        <v>41046</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="11">
+        <f t="shared" si="1"/>
+        <v>41047</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="11">
+        <f t="shared" si="1"/>
+        <v>41048</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="11">
+        <f t="shared" si="1"/>
+        <v>41049</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ca="1" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="11">
+        <f t="shared" si="1"/>
+        <v>41050</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="11">
+        <f t="shared" si="1"/>
+        <v>41051</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="11">
+        <f t="shared" si="1"/>
+        <v>41052</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="11">
+        <f t="shared" si="1"/>
+        <v>41053</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ca="1" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="11">
+        <f t="shared" si="1"/>
+        <v>41054</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="11">
+        <f t="shared" si="1"/>
+        <v>41055</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="11">
+        <f t="shared" si="1"/>
+        <v>41056</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="11">
+        <f t="shared" si="1"/>
+        <v>41057</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="11">
+        <f t="shared" si="1"/>
+        <v>41058</v>
+      </c>
+      <c r="B29">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="11">
+        <f t="shared" si="1"/>
+        <v>41059</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>